<commit_message>
home page test modified and added data supplier
</commit_message>
<xml_diff>
--- a/src/main/java/com/luma/testutil/LumaData.xlsx
+++ b/src/main/java/com/luma/testutil/LumaData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\eclipse-workspace\LUMA\src\main\java\com\luma\testutil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D226CF7A-B285-4E2B-9988-604934103759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EA9718-1B24-4856-A8E3-9FC66940663F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B5DACD30-F5D5-4982-BF6B-9441334A7FCC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B5DACD30-F5D5-4982-BF6B-9441334A7FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -450,15 +442,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E22A57CE-6810-498C-AEE7-4B6C6FB789B0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -466,7 +458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -488,20 +480,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184F7CB0-B5B4-4184-BEC4-868252004E38}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -518,7 +510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>

</xml_diff>